<commit_message>
hotfix double-encoding-issue by using triple-braces
</commit_message>
<xml_diff>
--- a/test/templates/Template.xlsx
+++ b/test/templates/Template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>{{AccountName__c}}（以下、甲という。）と　株式会社サンプル（以下、乙という。）は、</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>下記条件にて雇用契約を締結する。</t>
     <rPh sb="6" eb="8">
       <t>コヨウ</t>
@@ -89,42 +85,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">{{StartDateFormat__c}} 〜 {{EndDateFormat__c}}  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>{{Address__c}}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">{{JobDescription__c}} </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">{{StartTime__c}} 〜 {{EndTime__c}}  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">{{hasOverTime__c}} </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">{{HoliDayType__c}} </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>基本給(月)　{{Salary__c}}万円</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">{{DueDate__c}} </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">{{SalaryDate__c}} </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>下記に記名押印し、甲乙それぞれ１通づつ保管する。</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -145,11 +105,51 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>{{AccountName__c}}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>{{AccountAddress__c}}</t>
+    <t>{{{AccountName__c}}}（以下、甲という。）と　株式会社サンプル（以下、乙という。）は、</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{{{AccountAddress__c}}}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{{{AccountName__c}}}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">{{{StartDateFormat__c}}} 〜 {{{EndDateFormat__c}}}  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">{{{JobDescription__c}}} </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">{{{StartTime__c}}} 〜 {{{EndTime__c}}}  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{{{Address__c}}}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{{{hasOverTime__c}}}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">{{{HoliDayType__c}}} </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>基本給(月)　{{{Salary__c}}}万円</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">{{{DueDate__c}}} </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">{{{SalaryDate__c}}} </t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -482,15 +482,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -522,6 +513,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -919,7 +919,9 @@
   </sheetPr>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:H13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
@@ -946,15 +948,15 @@
     </row>
     <row r="2" spans="1:8" ht="25">
       <c r="A2" s="2"/>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2"/>
@@ -969,7 +971,7 @@
     <row r="4" spans="1:8">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -981,7 +983,7 @@
     <row r="5" spans="1:8">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1003,30 +1005,30 @@
     <row r="7" spans="1:8" ht="28" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="19"/>
+        <v>2</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
     </row>
     <row r="8" spans="1:8" ht="28" customHeight="1" thickBot="1">
       <c r="A8" s="2"/>
       <c r="B8" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="21"/>
+        <v>3</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="2"/>
@@ -1051,128 +1053,128 @@
     <row r="11" spans="1:8" ht="28" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="24"/>
+        <v>4</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
     </row>
     <row r="12" spans="1:8" ht="28" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="13"/>
+        <v>5</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="24"/>
     </row>
     <row r="13" spans="1:8" ht="28" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="13"/>
+        <v>6</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="28" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="13"/>
+        <v>7</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8" ht="28" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="13"/>
+        <v>8</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="24"/>
     </row>
     <row r="16" spans="1:8" ht="28" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="13"/>
+        <v>9</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8" ht="28" customHeight="1">
       <c r="A17" s="2"/>
       <c r="B17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="13"/>
+        <v>10</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="24"/>
     </row>
     <row r="18" spans="1:8" ht="28" customHeight="1">
       <c r="A18" s="2"/>
       <c r="B18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="13"/>
+        <v>11</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="24"/>
     </row>
     <row r="19" spans="1:8" ht="28" customHeight="1" thickBot="1">
       <c r="A19" s="2"/>
       <c r="B19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="16"/>
+        <v>12</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="2"/>
@@ -1187,7 +1189,7 @@
     <row r="21" spans="1:8">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1209,17 +1211,17 @@
     <row r="23" spans="1:8">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="9" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="10" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1237,13 +1239,13 @@
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="9" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="10" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:8">

</xml_diff>